<commit_message>
Added results, modified solvers.py
</commit_message>
<xml_diff>
--- a/Scripts/Results/Solutions_and_states.xlsx
+++ b/Scripts/Results/Solutions_and_states.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,10 +145,10 @@
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
@@ -176,6 +178,9 @@
       <c r="B3" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="D3" s="0" t="n">
         <v>819</v>
       </c>
@@ -190,6 +195,9 @@
       <c r="B4" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="D4" s="0" t="n">
         <v>13842</v>
       </c>
@@ -203,6 +211,9 @@
       </c>
       <c r="B5" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>83</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>11253</v>

</xml_diff>